<commit_message>
test: updated tests to that 'admin' is now returned if no user is set
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/settings_and_members.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/settings_and_members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8585CB-B44C-D54F-879C-E30443CA6502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9EC9D5-84F6-924F-95F0-E5875EC7752C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>tableName</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t>Viewer</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Manager</t>
   </si>
   <si>
     <t>table</t>
@@ -468,10 +462,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -485,9 +479,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -512,14 +506,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -529,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A745C3-9C92-3247-8929-D6B1D75D1CED}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -537,32 +523,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "fix[catalogue]: small bugfixes in ResourceDetails view"
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/settings_and_members.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/settings_and_members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9EC9D5-84F6-924F-95F0-E5875EC7752C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8585CB-B44C-D54F-879C-E30443CA6502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>tableName</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Viewer</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
   <si>
     <t>table</t>
@@ -462,10 +468,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -479,9 +485,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -506,6 +512,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -515,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A745C3-9C92-3247-8929-D6B1D75D1CED}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -523,32 +537,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "fix[catalogue]: small bugfixes in ResourceDetails view""
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/settings_and_members.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/settings_and_members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8585CB-B44C-D54F-879C-E30443CA6502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9EC9D5-84F6-924F-95F0-E5875EC7752C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>tableName</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t>Viewer</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Manager</t>
   </si>
   <si>
     <t>table</t>
@@ -468,10 +462,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -485,9 +479,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -512,14 +506,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -529,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A745C3-9C92-3247-8929-D6B1D75D1CED}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -537,32 +523,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: undo premature merge of feat/nopostgressuperuser
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/settings_and_members.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/settings_and_members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9EC9D5-84F6-924F-95F0-E5875EC7752C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8585CB-B44C-D54F-879C-E30443CA6502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>tableName</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Viewer</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
   <si>
     <t>table</t>
@@ -462,10 +468,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -479,9 +485,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -506,6 +512,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -515,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A745C3-9C92-3247-8929-D6B1D75D1CED}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -523,32 +537,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>